<commit_message>
Updated for file upload - removed optionsl cols
</commit_message>
<xml_diff>
--- a/backend/data/sample_questions/Complex_Numbers_MCQ.xlsx
+++ b/backend/data/sample_questions/Complex_Numbers_MCQ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soms/adaptive-assessment-system/backend/data/sample_questions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soumya.shrivastava/adaptive-assessment-system/backend/data/sample_questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C384CA-ACFE-D34C-8801-ECEA2CE2D9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF53450-8493-9742-B9E8-791D27834A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1272,7 +1272,7 @@
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>